<commit_message>
Put logick to separate thread, using Task.Run().
</commit_message>
<xml_diff>
--- a/DocFilesFillingProgramm/DocFilesFillingProgrammUI/bin/Debug/Storage/excelStorage.xlsx
+++ b/DocFilesFillingProgramm/DocFilesFillingProgrammUI/bin/Debug/Storage/excelStorage.xlsx
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="118">
   <si>
     <t>NAME</t>
   </si>
@@ -365,6 +365,222 @@
   </si>
   <si>
     <t>BLABLABLA</t>
+  </si>
+  <si>
+    <t>14</t>
+  </si>
+  <si>
+    <t>23.05.1997</t>
+  </si>
+  <si>
+    <t>02.12.2017</t>
+  </si>
+  <si>
+    <t>03.04.2018</t>
+  </si>
+  <si>
+    <t>04.04.2018</t>
+  </si>
+  <si>
+    <t>182</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>23.05.1998</t>
+  </si>
+  <si>
+    <t>02.12.2018</t>
+  </si>
+  <si>
+    <t>03.04.2019</t>
+  </si>
+  <si>
+    <t>04.04.2019</t>
+  </si>
+  <si>
+    <t>183</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>23.05.1999</t>
+  </si>
+  <si>
+    <t>02.12.2019</t>
+  </si>
+  <si>
+    <t>03.04.2020</t>
+  </si>
+  <si>
+    <t>04.04.2020</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>23.05.2000</t>
+  </si>
+  <si>
+    <t>02.12.2020</t>
+  </si>
+  <si>
+    <t>03.04.2021</t>
+  </si>
+  <si>
+    <t>04.04.2021</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>23.05.2001</t>
+  </si>
+  <si>
+    <t>02.12.2021</t>
+  </si>
+  <si>
+    <t>03.04.2022</t>
+  </si>
+  <si>
+    <t>04.04.2022</t>
+  </si>
+  <si>
+    <t>186</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>23.05.2002</t>
+  </si>
+  <si>
+    <t>02.12.2022</t>
+  </si>
+  <si>
+    <t>03.04.2023</t>
+  </si>
+  <si>
+    <t>04.04.2023</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>23.05.2003</t>
+  </si>
+  <si>
+    <t>02.12.2023</t>
+  </si>
+  <si>
+    <t>03.04.2024</t>
+  </si>
+  <si>
+    <t>04.04.2024</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>23.05.2004</t>
+  </si>
+  <si>
+    <t>02.12.2024</t>
+  </si>
+  <si>
+    <t>03.04.2025</t>
+  </si>
+  <si>
+    <t>04.04.2025</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23.05.2005</t>
+  </si>
+  <si>
+    <t>02.12.2025</t>
+  </si>
+  <si>
+    <t>03.04.2026</t>
+  </si>
+  <si>
+    <t>04.04.2026</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>23.05.2006</t>
+  </si>
+  <si>
+    <t>02.12.2026</t>
+  </si>
+  <si>
+    <t>03.04.2027</t>
+  </si>
+  <si>
+    <t>04.04.2027</t>
+  </si>
+  <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>23.05.2007</t>
+  </si>
+  <si>
+    <t>02.12.2027</t>
+  </si>
+  <si>
+    <t>03.04.2028</t>
+  </si>
+  <si>
+    <t>04.04.2028</t>
+  </si>
+  <si>
+    <t>192</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>23.05.2008</t>
+  </si>
+  <si>
+    <t>02.12.2028</t>
+  </si>
+  <si>
+    <t>03.04.2029</t>
+  </si>
+  <si>
+    <t>04.04.2029</t>
+  </si>
+  <si>
+    <t>193</t>
   </si>
 </sst>
 </file>
@@ -775,10 +991,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N3"/>
+  <dimension ref="A1:N15"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -916,7 +1132,7 @@
         <v>15</v>
       </c>
       <c r="K3" s="9">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>28</v>
@@ -926,6 +1142,534 @@
       </c>
       <c r="N3" s="9">
         <v>46</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A4" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="E4" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="F4" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K4" s="9">
+        <v>2</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="M4" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A5" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="B5" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="E5" s="9" t="s">
+        <v>54</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K5" s="9">
+        <v>2</v>
+      </c>
+      <c r="L5" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="M5" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="N5" s="9">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="9">
+        <v>2</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="N6" s="9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="9">
+        <v>2</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="N7" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="9">
+        <v>2</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="N8" s="9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="9">
+        <v>2</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="N9" s="9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="9">
+        <v>2</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="N10" s="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="9">
+        <v>2</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="N11" s="9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="9">
+        <v>2</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="N12" s="9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C13" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="9">
+        <v>2</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="N13" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="9">
+        <v>2</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="N14" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>6</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="9">
+        <v>2</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="N15" s="9">
+        <v>58</v>
       </c>
     </row>
   </sheetData>
@@ -939,31 +1683,31 @@
           <x14:formula1>
             <xm:f>SettingsSheet!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G3</xm:sqref>
+          <xm:sqref>G2:G15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>SettingsSheet!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H3</xm:sqref>
+          <xm:sqref>H2:H15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>SettingsSheet!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I3</xm:sqref>
+          <xm:sqref>I2:I15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>SettingsSheet!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J3</xm:sqref>
+          <xm:sqref>J2:J15</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>SettingsSheet!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K3</xm:sqref>
+          <xm:sqref>K2:K15</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Fix problem with hanging processes.
</commit_message>
<xml_diff>
--- a/DocFilesFillingProgramm/DocFilesFillingProgrammUI/bin/Debug/Storage/excelStorage.xlsx
+++ b/DocFilesFillingProgramm/DocFilesFillingProgrammUI/bin/Debug/Storage/excelStorage.xlsx
@@ -227,7 +227,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="401" uniqueCount="130">
   <si>
     <t>NAME</t>
   </si>
@@ -301,6 +301,48 @@
     <t>LASTNAME</t>
   </si>
   <si>
+    <t>ukrmark</t>
+  </si>
+  <si>
+    <t>germark</t>
+  </si>
+  <si>
+    <t>gender</t>
+  </si>
+  <si>
+    <t>dl</t>
+  </si>
+  <si>
+    <t>dn</t>
+  </si>
+  <si>
+    <t>filldate</t>
+  </si>
+  <si>
+    <t>hd</t>
+  </si>
+  <si>
+    <t>md</t>
+  </si>
+  <si>
+    <t>enddate</t>
+  </si>
+  <si>
+    <t>begindate</t>
+  </si>
+  <si>
+    <t>birthdate</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>KONSTANTIN</t>
+  </si>
+  <si>
+    <t>KOVALENKO</t>
+  </si>
+  <si>
     <t>13</t>
   </si>
   <si>
@@ -319,54 +361,6 @@
     <t>181</t>
   </si>
   <si>
-    <t>ukrmark</t>
-  </si>
-  <si>
-    <t>germark</t>
-  </si>
-  <si>
-    <t>gender</t>
-  </si>
-  <si>
-    <t>dl</t>
-  </si>
-  <si>
-    <t>dn</t>
-  </si>
-  <si>
-    <t>filldate</t>
-  </si>
-  <si>
-    <t>hd</t>
-  </si>
-  <si>
-    <t>md</t>
-  </si>
-  <si>
-    <t>enddate</t>
-  </si>
-  <si>
-    <t>begindate</t>
-  </si>
-  <si>
-    <t>birthdate</t>
-  </si>
-  <si>
-    <t>id</t>
-  </si>
-  <si>
-    <t>KONSTANTIN</t>
-  </si>
-  <si>
-    <t>DARYA</t>
-  </si>
-  <si>
-    <t>KOVALENKO</t>
-  </si>
-  <si>
-    <t>BLABLABLA</t>
-  </si>
-  <si>
     <t>14</t>
   </si>
   <si>
@@ -401,6 +395,228 @@
   </si>
   <si>
     <t>183</t>
+  </si>
+  <si>
+    <t>16</t>
+  </si>
+  <si>
+    <t>23.05.1999</t>
+  </si>
+  <si>
+    <t>02.12.2019</t>
+  </si>
+  <si>
+    <t>03.04.2020</t>
+  </si>
+  <si>
+    <t>04.04.2020</t>
+  </si>
+  <si>
+    <t>184</t>
+  </si>
+  <si>
+    <t>17</t>
+  </si>
+  <si>
+    <t>23.05.2000</t>
+  </si>
+  <si>
+    <t>02.12.2020</t>
+  </si>
+  <si>
+    <t>03.04.2021</t>
+  </si>
+  <si>
+    <t>04.04.2021</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>18</t>
+  </si>
+  <si>
+    <t>23.05.2001</t>
+  </si>
+  <si>
+    <t>02.12.2021</t>
+  </si>
+  <si>
+    <t>03.04.2022</t>
+  </si>
+  <si>
+    <t>04.04.2022</t>
+  </si>
+  <si>
+    <t>186</t>
+  </si>
+  <si>
+    <t>19</t>
+  </si>
+  <si>
+    <t>23.05.2002</t>
+  </si>
+  <si>
+    <t>02.12.2022</t>
+  </si>
+  <si>
+    <t>03.04.2023</t>
+  </si>
+  <si>
+    <t>04.04.2023</t>
+  </si>
+  <si>
+    <t>187</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>23.05.2003</t>
+  </si>
+  <si>
+    <t>02.12.2023</t>
+  </si>
+  <si>
+    <t>03.04.2024</t>
+  </si>
+  <si>
+    <t>04.04.2024</t>
+  </si>
+  <si>
+    <t>188</t>
+  </si>
+  <si>
+    <t>21</t>
+  </si>
+  <si>
+    <t>23.05.2004</t>
+  </si>
+  <si>
+    <t>02.12.2024</t>
+  </si>
+  <si>
+    <t>03.04.2025</t>
+  </si>
+  <si>
+    <t>04.04.2025</t>
+  </si>
+  <si>
+    <t>189</t>
+  </si>
+  <si>
+    <t>22</t>
+  </si>
+  <si>
+    <t>23.05.2005</t>
+  </si>
+  <si>
+    <t>02.12.2025</t>
+  </si>
+  <si>
+    <t>03.04.2026</t>
+  </si>
+  <si>
+    <t>04.04.2026</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>23.05.2006</t>
+  </si>
+  <si>
+    <t>02.12.2026</t>
+  </si>
+  <si>
+    <t>03.04.2027</t>
+  </si>
+  <si>
+    <t>04.04.2027</t>
+  </si>
+  <si>
+    <t>191</t>
+  </si>
+  <si>
+    <t>24</t>
+  </si>
+  <si>
+    <t>23.05.2007</t>
+  </si>
+  <si>
+    <t>02.12.2027</t>
+  </si>
+  <si>
+    <t>03.04.2028</t>
+  </si>
+  <si>
+    <t>04.04.2028</t>
+  </si>
+  <si>
+    <t>192</t>
+  </si>
+  <si>
+    <t>25</t>
+  </si>
+  <si>
+    <t>23.05.2008</t>
+  </si>
+  <si>
+    <t>02.12.2028</t>
+  </si>
+  <si>
+    <t>03.04.2029</t>
+  </si>
+  <si>
+    <t>04.04.2029</t>
+  </si>
+  <si>
+    <t>193</t>
+  </si>
+  <si>
+    <t>26</t>
+  </si>
+  <si>
+    <t>23.05.2009</t>
+  </si>
+  <si>
+    <t>02.12.2029</t>
+  </si>
+  <si>
+    <t>03.04.2030</t>
+  </si>
+  <si>
+    <t>04.04.2030</t>
+  </si>
+  <si>
+    <t>194</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>23.05.2010</t>
+  </si>
+  <si>
+    <t>02.12.2030</t>
+  </si>
+  <si>
+    <t>03.04.2031</t>
+  </si>
+  <si>
+    <t>04.04.2031</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>fsdfs</t>
+  </si>
+  <si>
+    <t>fsdf</t>
   </si>
 </sst>
 </file>
@@ -811,10 +1027,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N5"/>
+  <dimension ref="A1:N17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +1050,7 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B1" s="8" t="s">
         <v>0</v>
@@ -843,37 +1059,37 @@
         <v>23</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F1" s="8" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="N1" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="I1" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="J1" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
@@ -881,10 +1097,10 @@
         <v>22</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C2" s="9" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>18</v>
@@ -922,43 +1138,43 @@
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="9" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>43</v>
+        <v>128</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>45</v>
+        <v>129</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>25</v>
+        <v>39</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>26</v>
+        <v>40</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J3" s="9" t="s">
         <v>15</v>
       </c>
       <c r="K3" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="L3" s="9" t="s">
-        <v>28</v>
+        <v>42</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>29</v>
+        <v>43</v>
       </c>
       <c r="N3" s="9">
         <v>46</v>
@@ -966,31 +1182,31 @@
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="9">
+        <v>321423</v>
+      </c>
+      <c r="C4" s="9">
+        <v>423</v>
+      </c>
+      <c r="D4" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="E4" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D4" s="9" t="s">
+      <c r="F4" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="F4" s="9" t="s">
-        <v>49</v>
-      </c>
       <c r="G4" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H4" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I4" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J4" s="9" t="s">
         <v>15</v>
@@ -999,10 +1215,10 @@
         <v>2</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="N4" s="9">
         <v>47</v>
@@ -1010,31 +1226,31 @@
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="9">
+        <v>42</v>
+      </c>
+      <c r="C5" s="9">
+        <v>423</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="E5" s="9" t="s">
         <v>52</v>
       </c>
-      <c r="B5" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="C5" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D5" s="9" t="s">
+      <c r="F5" s="9" t="s">
         <v>53</v>
       </c>
-      <c r="E5" s="9" t="s">
-        <v>54</v>
-      </c>
-      <c r="F5" s="9" t="s">
-        <v>55</v>
-      </c>
       <c r="G5" s="9" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H5" s="9" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I5" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="J5" s="9" t="s">
         <v>15</v>
@@ -1043,13 +1259,541 @@
         <v>2</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="N5" s="9">
         <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A6" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B6" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="F6" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K6" s="9">
+        <v>1</v>
+      </c>
+      <c r="L6" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M6" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="N6" s="9">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A7" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="9">
+        <v>234</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F7" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K7" s="9">
+        <v>1</v>
+      </c>
+      <c r="L7" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="M7" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="N7" s="9">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A8" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C8" s="9">
+        <v>4</v>
+      </c>
+      <c r="D8" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E8" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="F8" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H8" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K8" s="9">
+        <v>1</v>
+      </c>
+      <c r="L8" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="M8" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="N8" s="9">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A9" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B9" s="9">
+        <v>4</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H9" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K9" s="9">
+        <v>1</v>
+      </c>
+      <c r="L9" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="M9" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="N9" s="9">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A10" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B10" s="9">
+        <v>3</v>
+      </c>
+      <c r="C10" s="9">
+        <v>423</v>
+      </c>
+      <c r="D10" s="9" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="F10" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J10" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K10" s="9">
+        <v>1</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>84</v>
+      </c>
+      <c r="M10" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="N10" s="9">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A11" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>87</v>
+      </c>
+      <c r="E11" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="F11" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K11" s="9">
+        <v>1</v>
+      </c>
+      <c r="L11" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="N11" s="9">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A12" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B12" s="9">
+        <v>23</v>
+      </c>
+      <c r="C12" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="E12" s="9" t="s">
+        <v>94</v>
+      </c>
+      <c r="F12" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12" s="9">
+        <v>1</v>
+      </c>
+      <c r="L12" s="9" t="s">
+        <v>96</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="N12" s="9">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A13" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C13" s="9">
+        <v>23</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="E13" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K13" s="9">
+        <v>1</v>
+      </c>
+      <c r="L13" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M13" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="N13" s="9">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A14" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C14" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="F14" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H14" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K14" s="9">
+        <v>1</v>
+      </c>
+      <c r="L14" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="N14" s="9">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A15" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B15" s="9">
+        <v>234</v>
+      </c>
+      <c r="C15" s="9">
+        <v>4</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="E15" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="F15" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K15" s="9">
+        <v>1</v>
+      </c>
+      <c r="L15" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="M15" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="N15" s="9">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A16" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C16" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="F16" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H16" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K16" s="9">
+        <v>1</v>
+      </c>
+      <c r="L16" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="M16" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="N16" s="9">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A17" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B17" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="9">
+        <v>4</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="E17" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="H17" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="K17" s="9">
+        <v>1</v>
+      </c>
+      <c r="L17" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="M17" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="N17" s="9">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -1063,31 +1807,31 @@
           <x14:formula1>
             <xm:f>SettingsSheet!$A$2:$A$4</xm:f>
           </x14:formula1>
-          <xm:sqref>G2:G5</xm:sqref>
+          <xm:sqref>G2:G17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>SettingsSheet!$B$2:$B$4</xm:f>
           </x14:formula1>
-          <xm:sqref>H2:H5</xm:sqref>
+          <xm:sqref>H2:H17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>SettingsSheet!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>I2:I5</xm:sqref>
+          <xm:sqref>I2:I17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>SettingsSheet!$D$2:$D$4</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J5</xm:sqref>
+          <xm:sqref>J2:J17</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>SettingsSheet!$E$2:$E$3</xm:f>
           </x14:formula1>
-          <xm:sqref>K2:K5</xm:sqref>
+          <xm:sqref>K2:K17</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>

<commit_message>
Embedded xlsx and docx files to logick dll. There is bug with interop doc, that i should fix.
</commit_message>
<xml_diff>
--- a/DocFilesFillingProgramm/DocFilesFillingProgrammUI/bin/Debug/Storage/excelStorage.xlsx
+++ b/DocFilesFillingProgramm/DocFilesFillingProgrammUI/bin/Debug/Storage/excelStorage.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8160"/>
   </bookViews>
   <sheets>
     <sheet name="ListSheet" sheetId="1" r:id="rId1"/>
@@ -337,10 +337,10 @@
     <t>id</t>
   </si>
   <si>
-    <t>KONSTANTIN</t>
-  </si>
-  <si>
-    <t>KOVALENKO</t>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Lastname</t>
   </si>
   <si>
     <t>13</t>
@@ -361,10 +361,10 @@
     <t>181</t>
   </si>
   <si>
-    <t>fsdfs</t>
-  </si>
-  <si>
-    <t>fsdf</t>
+    <t>Fem</t>
+  </si>
+  <si>
+    <t>ale</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -470,9 +470,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -778,10 +775,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:N3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -875,7 +872,7 @@
         <v>15</v>
       </c>
       <c r="K2" s="9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>21</v>
@@ -913,10 +910,10 @@
         <v>7</v>
       </c>
       <c r="I3" s="9" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="J3" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="K3" s="9">
         <v>1</v>
@@ -930,9 +927,6 @@
       <c r="N3" s="9">
         <v>46</v>
       </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="E11" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>